<commit_message>
added medications valuesets and improved overview
</commit_message>
<xml_diff>
--- a/StructureDefinition-ARFCondition.xlsx
+++ b/StructureDefinition-ARFCondition.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1469" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1468" uniqueCount="340">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-05-15T12:58:39+10:00</t>
+    <t>2024-05-15T15:51:17+10:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -619,7 +619,7 @@
     <t>Coding of the severity with a terminology is preferred, where possible.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/condition-severity</t>
+    <t>http://fhir-arf-register.nardhc.org/ValueSet/arf-severity-vs</t>
   </si>
   <si>
     <t>&lt; 272141005 |Severities|</t>
@@ -3148,13 +3148,13 @@
       </c>
       <c r="E15" s="2"/>
       <c r="F15" t="s" s="2">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="G15" t="s" s="2">
         <v>88</v>
       </c>
       <c r="H15" t="s" s="2">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="I15" t="s" s="2">
         <v>76</v>
@@ -3198,11 +3198,9 @@
         <v>76</v>
       </c>
       <c r="X15" t="s" s="2">
-        <v>112</v>
-      </c>
-      <c r="Y15" t="s" s="2">
-        <v>191</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="Y15" s="2"/>
       <c r="Z15" t="s" s="2">
         <v>193</v>
       </c>

</xml_diff>